<commit_message>
amended the furnace grop dict, made datafolder updates
</commit_message>
<xml_diff>
--- a/import_data/CAPEX OPEX Per Technology.xlsx
+++ b/import_data/CAPEX OPEX Per Technology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{D1A03796-A78E-4FC3-9712-F10AC328032A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92227F77-9713-46D3-8EF4-5B0C2B2125CA}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{D1A03796-A78E-4FC3-9712-F10AC328032A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCD1C5DA-3B42-475E-9FD7-CF25EB1454D0}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" activeTab="1" xr2:uid="{5B88B727-8630-4BCE-A967-4A2C273300FC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5B88B727-8630-4BCE-A967-4A2C273300FC}"/>
   </bookViews>
   <sheets>
     <sheet name="GF capex" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,10 @@
     <t>BAT BF-BOF_bio PCI</t>
   </si>
   <si>
-    <t>BAT BF-BOF+CCS</t>
-  </si>
-  <si>
-    <t>Smelting Reduction+CCS</t>
-  </si>
-  <si>
     <t>Charcoal mini furnace</t>
   </si>
   <si>
     <t>Electrolyzer-EAF</t>
-  </si>
-  <si>
-    <t>DRI-EAF+CCS</t>
   </si>
   <si>
     <t>DRI-EAF_100% green H2</t>
@@ -92,16 +83,10 @@
     <t>BAT BF-BOF+CCUS</t>
   </si>
   <si>
-    <t>DRI-Melt-BOF+CCS</t>
-  </si>
-  <si>
     <t>DRI-Melt-BOF_100% zero-C H2</t>
   </si>
   <si>
     <t>Electrowinning-EAF</t>
-  </si>
-  <si>
-    <t>BAT BF-BOF+BECCS</t>
   </si>
   <si>
     <t>Initial</t>
@@ -123,6 +108,21 @@
   </si>
   <si>
     <t>Technology type</t>
+  </si>
+  <si>
+    <t>Smelting Reduction+CCUS</t>
+  </si>
+  <si>
+    <t>BAT BF-BOF+BECCUS</t>
+  </si>
+  <si>
+    <t>DRI-Melt-BOF+CCUS</t>
+  </si>
+  <si>
+    <t>BAT BF-BOF+CCU</t>
+  </si>
+  <si>
+    <t>DRI-EAF+CCUS</t>
   </si>
 </sst>
 </file>
@@ -477,17 +477,17 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.8203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -583,7 +583,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -681,7 +681,7 @@
         <v>871.85064220183472</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -779,7 +779,7 @@
         <v>1066.8506422018347</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -877,7 +877,7 @@
         <v>698.34183486238533</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -975,7 +975,7 @@
         <v>357.7963864282209</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>603.34183486238533</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>698.34183486238533</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>698.34183486238533</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>1066.8506422018347</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1465,9 +1465,9 @@
         <v>1066.8506422018347</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>1230.0944923998388</v>
@@ -1563,9 +1563,9 @@
         <v>1188.37661957146</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>646.13638642822093</v>
@@ -1661,9 +1661,9 @@
         <v>404.46638642822091</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>206.07533632286996</v>
@@ -1759,9 +1759,9 @@
         <v>206.07533632286996</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>709.87</v>
@@ -1857,9 +1857,9 @@
         <v>662.34</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>843.10492686238535</v>
@@ -1955,9 +1955,9 @@
         <v>752.22587466238531</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>698.34183486238533</v>
@@ -2053,9 +2053,9 @@
         <v>698.34183486238533</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2151,9 +2151,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>210</v>
@@ -2249,9 +2249,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>1298.549525531806</v>
@@ -2347,9 +2347,9 @@
         <v>1239.3375886808133</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>666.58592520512366</v>
@@ -2445,9 +2445,9 @@
         <v>650.42354656197949</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>603.34183486238533</v>
@@ -2543,9 +2543,9 @@
         <v>603.34183486238533</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>744.6</v>
@@ -2641,9 +2641,9 @@
         <v>652.79999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>1279.3610678419107</v>
@@ -2748,30 +2748,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F3D0DF-0035-4729-81FE-EF9D246469F5}">
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1">
         <v>2020</v>
@@ -2867,7 +2867,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>2030</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>187.5</v>
@@ -2974,7 +2974,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>2030</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>285</v>
@@ -3081,7 +3081,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>2030</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>186.55603236551863</v>
@@ -3188,7 +3188,7 @@
         <v>186.55603236551863</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>2030</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>160.14230424929596</v>
@@ -3295,7 +3295,7 @@
         <v>95.582236255289374</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>2030</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>161.17759706353402</v>
@@ -3402,7 +3402,7 @@
         <v>161.17759706353402</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>2030</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>186.55603236551863</v>
@@ -3509,7 +3509,7 @@
         <v>186.55603236551863</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>2030</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>186.55603236551863</v>
@@ -3616,7 +3616,7 @@
         <v>186.55603236551863</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>2030</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E9">
         <v>285</v>
@@ -3723,7 +3723,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>2030</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E10">
         <v>285</v>
@@ -3830,9 +3830,9 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>2028</v>
@@ -3841,7 +3841,7 @@
         <v>2070</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E11">
         <v>328.60919463891491</v>
@@ -3937,9 +3937,9 @@
         <v>317.46462267563663</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>2028</v>
@@ -3948,7 +3948,7 @@
         <v>2070</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E12">
         <v>172.60979451817616</v>
@@ -4044,9 +4044,9 @@
         <v>108.0497265241696</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>2051</v>
@@ -4055,7 +4055,7 @@
         <v>2070</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>44.318514766423839</v>
@@ -4151,9 +4151,9 @@
         <v>44.318514766423839</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>2035</v>
@@ -4162,7 +4162,7 @@
         <v>2070</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E14">
         <v>189.63568281915599</v>
@@ -4258,9 +4258,9 @@
         <v>176.93845092543677</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>2025</v>
@@ -4269,7 +4269,7 @@
         <v>2070</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>225.22825093854229</v>
@@ -4365,9 +4365,9 @@
         <v>200.95069150103299</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>2028</v>
@@ -4376,7 +4376,7 @@
         <v>2070</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>186.55603236551863</v>
@@ -4472,9 +4472,9 @@
         <v>186.55603236551863</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>2020</v>
@@ -4483,7 +4483,7 @@
         <v>2070</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -4579,9 +4579,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>2020</v>
@@ -4590,7 +4590,7 @@
         <v>2070</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E18">
         <v>125.411</v>
@@ -4686,9 +4686,9 @@
         <v>125.411</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>2028</v>
@@ -4697,7 +4697,7 @@
         <v>2070</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E19">
         <v>346.89636968559745</v>
@@ -4793,9 +4793,9 @@
         <v>331.07840854372256</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>2028</v>
@@ -4804,7 +4804,7 @@
         <v>2070</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E20">
         <v>178.07271343191354</v>
@@ -4900,9 +4900,9 @@
         <v>173.75507258221657</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>2028</v>
@@ -4911,7 +4911,7 @@
         <v>2070</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E21">
         <v>161.17759706353402</v>
@@ -5007,9 +5007,9 @@
         <v>161.17759706353402</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>2035</v>
@@ -5018,7 +5018,7 @@
         <v>2070</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E22">
         <v>198.91350448271311</v>
@@ -5114,9 +5114,9 @@
         <v>174.38992173826901</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>2028</v>
@@ -5125,7 +5125,7 @@
         <v>2070</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E23">
         <v>341.77033776951453</v>
@@ -5230,18 +5230,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DCA1AF-7FFF-485C-ACA8-5A2E538B55BD}">
   <dimension ref="A1:AF23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -5337,7 +5337,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>123.67359046905142</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>129.7454074415285</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>118.2709560009595</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>107.6672142896653</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>115.31289132206044</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>118.2709560009595</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>118.2709560009595</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>129.7454074415285</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -6219,9 +6219,9 @@
         <v>129.7454074415285</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>183.80157163059505</v>
@@ -6317,9 +6317,9 @@
         <v>182.50258040856943</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>116.64540765296805</v>
@@ -6415,9 +6415,9 @@
         <v>109.12040248507815</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>123.67359046905142</v>
@@ -6513,9 +6513,9 @@
         <v>123.67359046905142</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>118.62991450733945</v>
@@ -6611,9 +6611,9 @@
         <v>117.14994804220183</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>144.49298389836392</v>
@@ -6709,9 +6709,9 @@
         <v>141.66323532610448</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>118.2709560009595</v>
@@ -6807,9 +6807,9 @@
         <v>118.2709560009595</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>526.20000000000005</v>
@@ -6905,9 +6905,9 @@
         <v>526.20000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>62.986140000000006</v>
@@ -7003,9 +7003,9 @@
         <v>62.986140000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>139.03817460704778</v>
@@ -7101,9 +7101,9 @@
         <v>137.19446156527806</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>136.25538273848147</v>
@@ -7199,9 +7199,9 @@
         <v>135.75212630278384</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>115.31289132206044</v>
@@ -7297,9 +7297,9 @@
         <v>115.31289132206044</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>119.71132067889909</v>
@@ -7395,9 +7395,9 @@
         <v>116.8528960733945</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>200.11558338601148</v>
@@ -7499,31 +7499,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="f6f44a7d-d6f5-4042-8792-19cb5f90fb06">
-      <UserInfo>
-        <DisplayName>Andrew Isabirye</DisplayName>
-        <AccountId>30706</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f94796c5baa2ef88ac6145701948dc8f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e880ceb9264c792c54763cc60e020778" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="319a675c9647c7594acaff66597be50a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88dc2720d39439db86350823647c6b2d" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
     <xsd:import namespace="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
     <xsd:element name="properties">
@@ -7536,6 +7513,12 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7554,6 +7537,40 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -7686,14 +7703,31 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="f6f44a7d-d6f5-4042-8792-19cb5f90fb06">
+      <UserInfo>
+        <DisplayName>Andrew Isabirye</DisplayName>
+        <AccountId>30706</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{052113BB-1538-4519-B445-D847E39824EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{621E4A8A-3A20-4BCE-A4A6-D2B9AEED33CE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7705,20 +7739,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C067B80A-8597-4D34-B156-6FC444C61735}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{052113BB-1538-4519-B445-D847E39824EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>